<commit_message>
end of pilot changes
</commit_message>
<xml_diff>
--- a/app/config/tables/MIF_V_OOP/forms/MIF_V_OOP/MIF_V_OOP.xlsx
+++ b/app/config/tables/MIF_V_OOP/forms/MIF_V_OOP/MIF_V_OOP.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A601D0-C1A9-4A9C-A7EF-C0192FC301BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E147E51-4DF0-40D7-942A-460FB0B21F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="728" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="728" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="220">
   <si>
     <t>setting_name</t>
   </si>
@@ -593,24 +593,12 @@
     <t>Prestação de serviços (pagamentos alem de materiais, diagnosticos e medicamentos)</t>
   </si>
   <si>
-    <t>data("OOP_B_OUTT") != null || data("OOP_B_OUTQ") ==0</t>
-  </si>
-  <si>
     <t>Nemhuma</t>
   </si>
   <si>
     <t>Nemhuma destes</t>
   </si>
   <si>
-    <t xml:space="preserve">data("OOP_B_TRAQ")!=null </t>
-  </si>
-  <si>
-    <t>data("OOP_B_TRAM")!=null ||data("OOP_B_TRAQ")==0</t>
-  </si>
-  <si>
-    <t>data("OOP_B_TRAM_OU")!=null ||data("OOP_B_TRAQ")==0</t>
-  </si>
-  <si>
     <t xml:space="preserve">Caterther </t>
   </si>
   <si>
@@ -656,9 +644,6 @@
     <t>Quanto é que pagou pelos outros despesas?</t>
   </si>
   <si>
-    <t xml:space="preserve">Quanto é que pagou pelo transporte de/para o estabelecimento de saúde (ida e volta)? </t>
-  </si>
-  <si>
     <t>Observações</t>
   </si>
   <si>
@@ -675,6 +660,51 @@
   </si>
   <si>
     <t>Carro de Transporte</t>
+  </si>
+  <si>
+    <t>data("OOP_B_OUTT") != null || data("OOP_B_OUTQ") ==0 || data("OOP_BIRTH") != "1"</t>
+  </si>
+  <si>
+    <t>Partos domiciliar: Incluindo multas</t>
+  </si>
+  <si>
+    <t>Incluindo multas se for parto domicilar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se for multado naaltura de vacinacao evite conta duplo </t>
+  </si>
+  <si>
+    <t>OOP_B_TRAQ_COMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voce: Quanto é que pagou pelo transporte de/para o estabelecimento de saúde (ida e volta)? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acompanhantes: Quanto é que pagou pelo transporte de/para o estabelecimento de saúde (ida e volta)? </t>
+  </si>
+  <si>
+    <t>Did (at least part of the birth) take place in a health facility?</t>
+  </si>
+  <si>
+    <t>Foi (pelo menos parte de) o parto numa estabelecimento de saude?</t>
+  </si>
+  <si>
+    <t>OOP_FACILITY</t>
+  </si>
+  <si>
+    <t>data("OOP_FACILITY") != null</t>
+  </si>
+  <si>
+    <t>data("OOP_FACILITY")!="2"</t>
+  </si>
+  <si>
+    <t>data("OOP_B_TRAQ")!=null ||data("OOP_FACILITY")!="2"</t>
+  </si>
+  <si>
+    <t>data("OOP_B_TRAM")!=null ||data("OOP_B_TRAQ")==0 || data("OOP_FACILITY")!="2"</t>
+  </si>
+  <si>
+    <t>data("OOP_B_TRAM_OU")!=null ||data("OOP_B_TRAQ")==0 || data("OOP_FACILITY")!="2"</t>
   </si>
 </sst>
 </file>
@@ -1239,11 +1269,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
-  <dimension ref="A1:T57"/>
+  <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1350,61 +1380,64 @@
         <v>108</v>
       </c>
       <c r="H3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="K3" t="s">
         <v>172</v>
       </c>
+      <c r="M3" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>214</v>
+      </c>
+      <c r="G4" t="s">
+        <v>212</v>
+      </c>
+      <c r="H4" t="s">
+        <v>213</v>
+      </c>
+      <c r="K4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A5" s="16"/>
-      <c r="B5" t="s">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" s="16"/>
+      <c r="B6" t="s">
         <v>55</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A6" s="15"/>
-      <c r="B6" t="s">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="15"/>
+      <c r="B7" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" t="s">
-        <v>82</v>
-      </c>
-      <c r="H7" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F8" t="s">
-        <v>87</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>181</v>
+        <v>82</v>
       </c>
       <c r="H8" t="s">
-        <v>196</v>
-      </c>
-      <c r="K8" t="s">
-        <v>126</v>
-      </c>
-      <c r="M8" t="s">
-        <v>205</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.35">
@@ -1412,97 +1445,112 @@
         <v>45</v>
       </c>
       <c r="F9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" t="s">
+        <v>181</v>
+      </c>
+      <c r="H9" t="s">
+        <v>192</v>
+      </c>
+      <c r="K9" t="s">
+        <v>126</v>
+      </c>
+      <c r="M9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s">
         <v>88</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G10" t="s">
         <v>85</v>
       </c>
-      <c r="H9" t="s">
-        <v>197</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="H10" t="s">
+        <v>193</v>
+      </c>
+      <c r="K10" t="s">
         <v>129</v>
       </c>
-      <c r="M9" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
+      <c r="M10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
         <v>86</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="D11" t="s">
-        <v>123</v>
-      </c>
-      <c r="E11" t="s">
-        <v>133</v>
-      </c>
-      <c r="F11" t="s">
-        <v>130</v>
-      </c>
-      <c r="G11" t="s">
-        <v>145</v>
-      </c>
-      <c r="H11" t="s">
-        <v>92</v>
-      </c>
-      <c r="K11" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" t="s">
+        <v>145</v>
+      </c>
+      <c r="H12" t="s">
+        <v>92</v>
+      </c>
+      <c r="K12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
         <v>46</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>47</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>131</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>146</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H13" t="s">
         <v>179</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K13" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
         <v>86</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="D15" t="s">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="D16" t="s">
         <v>54</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F16" t="s">
         <v>89</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G16" t="s">
         <v>91</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H16" t="s">
         <v>92</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K16" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.35">
@@ -1512,127 +1560,119 @@
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15" t="s">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" t="s">
+      <c r="E21" s="15"/>
+      <c r="F21" t="s">
         <v>93</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" t="s">
         <v>180</v>
       </c>
-      <c r="H20" t="s">
-        <v>198</v>
-      </c>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="L20" s="15"/>
-      <c r="M20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B21" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
+      <c r="H21" t="s">
+        <v>194</v>
+      </c>
       <c r="I21" s="15"/>
       <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
+      <c r="K21" s="15" t="s">
+        <v>137</v>
+      </c>
       <c r="L21" s="15"/>
+      <c r="M21" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>207</v>
-      </c>
+      <c r="B22" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
       <c r="I22" s="15"/>
       <c r="J22" s="15"/>
-      <c r="K22" s="15" t="s">
-        <v>175</v>
-      </c>
+      <c r="K22" s="15"/>
       <c r="L22" s="15"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15" t="s">
-        <v>46</v>
+        <v>123</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>47</v>
+        <v>157</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="I23" s="15"/>
       <c r="J23" s="15"/>
       <c r="K23" s="15" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L23" s="15"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B24" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>195</v>
+      </c>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
+      <c r="K24" s="15" t="s">
+        <v>176</v>
+      </c>
       <c r="L24" s="15"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
+      <c r="B25" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>140</v>
+      </c>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -1646,39 +1686,37 @@
     <row r="26" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
-      <c r="D26" s="15" t="s">
-        <v>54</v>
-      </c>
+      <c r="D26" s="15"/>
       <c r="E26" s="15"/>
-      <c r="F26" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="G26" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="H26" s="15" t="s">
-        <v>200</v>
-      </c>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
       <c r="I26" s="15"/>
       <c r="J26" s="15"/>
-      <c r="K26" s="15" t="s">
-        <v>163</v>
-      </c>
+      <c r="K26" s="15"/>
       <c r="L26" s="15"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B27" s="15" t="s">
-        <v>56</v>
-      </c>
+      <c r="B27" s="15"/>
       <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
+      <c r="D27" s="15" t="s">
+        <v>54</v>
+      </c>
       <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="15"/>
+      <c r="F27" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>196</v>
+      </c>
       <c r="I27" s="15"/>
       <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
+      <c r="K27" s="15" t="s">
+        <v>163</v>
+      </c>
       <c r="L27" s="15"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.35">
@@ -1698,7 +1736,7 @@
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B29" s="15" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
@@ -1713,7 +1751,7 @@
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B30" s="15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
@@ -1727,118 +1765,120 @@
       <c r="L30" s="15"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17" t="s">
+      <c r="B31" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17" t="s">
+      <c r="E32" s="17"/>
+      <c r="F32" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="G31" s="17" t="s">
+      <c r="G32" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="H31" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="L31" s="17"/>
-      <c r="M31" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B32" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
+      <c r="H32" s="17" t="s">
+        <v>197</v>
+      </c>
       <c r="I32" s="17"/>
       <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
+      <c r="K32" s="17" t="s">
+        <v>141</v>
+      </c>
       <c r="L32" s="17"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="G33" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="H33" s="17" t="s">
-        <v>97</v>
-      </c>
+      <c r="M32" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B33" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
       <c r="I33" s="17"/>
       <c r="J33" s="17"/>
-      <c r="K33" s="17" t="s">
-        <v>177</v>
-      </c>
+      <c r="K33" s="17"/>
       <c r="L33" s="17"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
       <c r="D34" s="17" t="s">
-        <v>46</v>
+        <v>123</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>47</v>
+        <v>150</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H34" s="17" t="s">
-        <v>152</v>
+        <v>97</v>
       </c>
       <c r="I34" s="17"/>
       <c r="J34" s="17"/>
       <c r="K34" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L34" s="17"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B35" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>152</v>
+      </c>
       <c r="I35" s="17"/>
       <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
+      <c r="K35" s="17" t="s">
+        <v>178</v>
+      </c>
       <c r="L35" s="17"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B36" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>144</v>
+      </c>
       <c r="D36" s="17"/>
       <c r="E36" s="17"/>
       <c r="F36" s="17"/>
@@ -1849,45 +1889,43 @@
       <c r="K36" s="17"/>
       <c r="L36" s="17"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
-      <c r="D37" s="17" t="s">
-        <v>54</v>
-      </c>
+      <c r="D37" s="17"/>
       <c r="E37" s="17"/>
-      <c r="F37" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="G37" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="H37" s="17" t="s">
-        <v>97</v>
-      </c>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
       <c r="I37" s="17"/>
       <c r="J37" s="17"/>
-      <c r="K37" s="17" t="s">
-        <v>162</v>
-      </c>
+      <c r="K37" s="17"/>
       <c r="L37" s="17"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B38" s="17" t="s">
-        <v>56</v>
-      </c>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B38" s="17"/>
       <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
+      <c r="D38" s="17" t="s">
+        <v>54</v>
+      </c>
       <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
+      <c r="F38" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="H38" s="17" t="s">
+        <v>97</v>
+      </c>
       <c r="I38" s="17"/>
       <c r="J38" s="17"/>
-      <c r="K38" s="17"/>
+      <c r="K38" s="17" t="s">
+        <v>162</v>
+      </c>
       <c r="L38" s="17"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B39" s="17" t="s">
         <v>56</v>
       </c>
@@ -1902,9 +1940,9 @@
       <c r="K39" s="17"/>
       <c r="L39" s="17"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B40" s="17" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
@@ -1917,9 +1955,9 @@
       <c r="K40" s="17"/>
       <c r="L40" s="17"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B41" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C41" s="17"/>
       <c r="D41" s="17"/>
@@ -1932,205 +1970,271 @@
       <c r="K41" s="17"/>
       <c r="L41" s="17"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18" t="s">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B42" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="17"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18" t="s">
+      <c r="E43" s="18"/>
+      <c r="F43" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G43" t="s">
         <v>99</v>
       </c>
-      <c r="H42" t="s">
-        <v>202</v>
-      </c>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="L42" s="18"/>
-      <c r="M42" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B43" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
+      <c r="H43" t="s">
+        <v>198</v>
+      </c>
       <c r="I43" s="18"/>
       <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
+      <c r="K43" s="18" t="s">
+        <v>154</v>
+      </c>
       <c r="L43" s="18"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18" t="s">
-        <v>54</v>
-      </c>
+      <c r="M43" t="s">
+        <v>200</v>
+      </c>
+      <c r="O43" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B44" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D44" s="18"/>
       <c r="E44" s="18"/>
-      <c r="F44" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="G44" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="H44" s="18" t="s">
-        <v>156</v>
-      </c>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
       <c r="I44" s="18"/>
       <c r="J44" s="18"/>
-      <c r="K44" s="18" t="s">
-        <v>182</v>
-      </c>
+      <c r="K44" s="18"/>
       <c r="L44" s="18"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B45" s="18" t="s">
-        <v>56</v>
-      </c>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B45" s="18"/>
       <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
+      <c r="D45" s="18" t="s">
+        <v>35</v>
+      </c>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
       <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
+      <c r="H45" s="18" t="s">
+        <v>208</v>
+      </c>
       <c r="I45" s="18"/>
       <c r="J45" s="18"/>
       <c r="K45" s="18"/>
       <c r="L45" s="18"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B46" s="18" t="s">
-        <v>38</v>
-      </c>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B46" s="18"/>
       <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
+      <c r="D46" s="18" t="s">
+        <v>54</v>
+      </c>
       <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
+      <c r="F46" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="G46" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>156</v>
+      </c>
       <c r="I46" s="18"/>
       <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
+      <c r="K46" s="18" t="s">
+        <v>205</v>
+      </c>
       <c r="L46" s="18"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A47" s="16"/>
-      <c r="B47" t="s">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B47" s="18" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B48" t="s">
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B48" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A49" s="16"/>
+      <c r="B49" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A50" s="16"/>
+      <c r="B50" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D49" t="s">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D52" t="s">
         <v>35</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G52" t="s">
         <v>121</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H52" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D50" t="s">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D53" t="s">
         <v>45</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F53" t="s">
         <v>112</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G53" t="s">
         <v>100</v>
       </c>
-      <c r="H50" t="s">
-        <v>203</v>
-      </c>
-      <c r="K50" t="s">
-        <v>185</v>
-      </c>
-      <c r="M50" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D52" t="s">
+      <c r="H53" t="s">
+        <v>210</v>
+      </c>
+      <c r="K53" t="s">
+        <v>217</v>
+      </c>
+      <c r="M53" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D55" t="s">
         <v>123</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E55" t="s">
         <v>102</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F55" t="s">
         <v>113</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G55" t="s">
         <v>101</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H55" t="s">
         <v>101</v>
       </c>
-      <c r="K52" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D53" t="s">
+      <c r="K55" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D56" t="s">
         <v>114</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E56" t="s">
         <v>168</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F56" t="s">
         <v>167</v>
       </c>
-      <c r="K53" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B54" t="s">
+      <c r="K56" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D57" t="s">
+        <v>45</v>
+      </c>
+      <c r="F57" t="s">
+        <v>209</v>
+      </c>
+      <c r="G57" t="s">
+        <v>100</v>
+      </c>
+      <c r="H57" t="s">
+        <v>211</v>
+      </c>
+      <c r="K57" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B55" t="s">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D56" t="s">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D60" t="s">
         <v>54</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F60" t="s">
         <v>165</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G60" t="s">
         <v>166</v>
       </c>
-      <c r="H56" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B57" t="s">
+      <c r="H60" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B62" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2143,9 +2247,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2257,7 +2361,7 @@
         <v>105</v>
       </c>
       <c r="D8" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -2302,7 +2406,7 @@
         <v>107</v>
       </c>
       <c r="D11" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -2344,10 +2448,10 @@
         <v>77</v>
       </c>
       <c r="C14" t="s">
+        <v>182</v>
+      </c>
+      <c r="D14" t="s">
         <v>183</v>
-      </c>
-      <c r="D14" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -2362,7 +2466,7 @@
         <v>169</v>
       </c>
       <c r="D16" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -2389,10 +2493,10 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D19" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -2485,7 +2589,7 @@
         <v>170</v>
       </c>
       <c r="D26" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -2500,7 +2604,7 @@
         <v>171</v>
       </c>
       <c r="D27" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -2580,7 +2684,7 @@
         <v>159</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -2610,7 +2714,7 @@
         <v>161</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
@@ -3054,9 +3158,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3257,6 +3361,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>214</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>165</v>
@@ -3265,6 +3380,17 @@
         <v>54</v>
       </c>
       <c r="C26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>209</v>
+      </c>
+      <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
end of pilot changes2
</commit_message>
<xml_diff>
--- a/app/config/tables/MIF_V_OOP/forms/MIF_V_OOP/MIF_V_OOP.xlsx
+++ b/app/config/tables/MIF_V_OOP/forms/MIF_V_OOP/MIF_V_OOP.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E147E51-4DF0-40D7-942A-460FB0B21F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1933490E-B281-4857-B421-0D3411B64DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="728" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="728" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="221">
   <si>
     <t>setting_name</t>
   </si>
@@ -656,9 +656,6 @@
     <t>Quais diagnósticos? (diagnósticos/exames/análises)</t>
   </si>
   <si>
-    <t>Você pagou pelo parto? (Prestacao de servico, materiais, diagnosticos, medicamentos)</t>
-  </si>
-  <si>
     <t>Carro de Transporte</t>
   </si>
   <si>
@@ -686,9 +683,6 @@
     <t>Did (at least part of the birth) take place in a health facility?</t>
   </si>
   <si>
-    <t>Foi (pelo menos parte de) o parto numa estabelecimento de saude?</t>
-  </si>
-  <si>
     <t>OOP_FACILITY</t>
   </si>
   <si>
@@ -705,6 +699,15 @@
   </si>
   <si>
     <t>data("OOP_B_TRAM_OU")!=null ||data("OOP_B_TRAQ")==0 || data("OOP_FACILITY")!="2"</t>
+  </si>
+  <si>
+    <t>O parto foi num estabelecimento de saude? (pelo menos um parte)</t>
+  </si>
+  <si>
+    <t>Você pagou pelo parto? &lt;br&gt; (Prestacao de servico, materiais, diagnosticos, medicamentos)</t>
+  </si>
+  <si>
+    <t>data("OOP_B_TRAM_COMP")!=null ||data("OOP_B_TRAQ")==0 || data("OOP_FACILITY")!="2"</t>
   </si>
 </sst>
 </file>
@@ -1271,9 +1274,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5FB9AA-D433-6046-85E1-401DEB18B3FD}">
   <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F57" sqref="F57"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1380,13 +1383,13 @@
         <v>108</v>
       </c>
       <c r="H3" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="K3" t="s">
         <v>172</v>
       </c>
       <c r="M3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
@@ -1397,16 +1400,16 @@
         <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H4" t="s">
+        <v>218</v>
+      </c>
+      <c r="K4" t="s">
         <v>213</v>
-      </c>
-      <c r="K4" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
@@ -2011,7 +2014,7 @@
         <v>200</v>
       </c>
       <c r="O43" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.35">
@@ -2041,7 +2044,7 @@
       <c r="F45" s="18"/>
       <c r="G45" s="18"/>
       <c r="H45" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I45" s="18"/>
       <c r="J45" s="18"/>
@@ -2067,7 +2070,7 @@
       <c r="I46" s="18"/>
       <c r="J46" s="18"/>
       <c r="K46" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L46" s="18"/>
     </row>
@@ -2113,7 +2116,7 @@
         <v>55</v>
       </c>
       <c r="C50" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.35">
@@ -2143,10 +2146,10 @@
         <v>100</v>
       </c>
       <c r="H53" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K53" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="M53" t="s">
         <v>201</v>
@@ -2169,7 +2172,7 @@
         <v>101</v>
       </c>
       <c r="K55" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.35">
@@ -2183,7 +2186,7 @@
         <v>167</v>
       </c>
       <c r="K56" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.35">
@@ -2191,16 +2194,16 @@
         <v>45</v>
       </c>
       <c r="F57" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G57" t="s">
         <v>100</v>
       </c>
       <c r="H57" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K57" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.35">
@@ -2361,7 +2364,7 @@
         <v>105</v>
       </c>
       <c r="D8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -3158,8 +3161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -3363,7 +3366,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B24" t="s">
         <v>46</v>
@@ -3385,7 +3388,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B27" t="s">
         <v>45</v>

</xml_diff>